<commit_message>
Introduction and Primary Setup
</commit_message>
<xml_diff>
--- a/Typescript.xlsx
+++ b/Typescript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\KAIZEN\Typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8145BF98-5F06-4946-8567-6F672012860E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAACC426-5092-45AD-96D3-91BE15C9C30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t>Typescript</t>
   </si>
@@ -338,13 +338,91 @@
   </si>
   <si>
     <t>The Course Project Setup</t>
+  </si>
+  <si>
+    <t>Module Introduction</t>
+  </si>
+  <si>
+    <t>Using Types</t>
+  </si>
+  <si>
+    <t>Typescript Types and Javascript Types</t>
+  </si>
+  <si>
+    <t>Important Typecasting</t>
+  </si>
+  <si>
+    <t>Working with Numbers String and Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type Assignment and Type Interface </t>
+  </si>
+  <si>
+    <t>Quiz 1: Understanding Types</t>
+  </si>
+  <si>
+    <t>Object Types</t>
+  </si>
+  <si>
+    <t>Nested Object and Types</t>
+  </si>
+  <si>
+    <t>Array Types</t>
+  </si>
+  <si>
+    <t>Working with Tuples</t>
+  </si>
+  <si>
+    <t>Working with Enums</t>
+  </si>
+  <si>
+    <t>The 'any' type</t>
+  </si>
+  <si>
+    <t>Union Types</t>
+  </si>
+  <si>
+    <t>Literal Types</t>
+  </si>
+  <si>
+    <t>Type Aliases/Custom Types</t>
+  </si>
+  <si>
+    <t>Type Aliases &amp; Object Types</t>
+  </si>
+  <si>
+    <t>Quiz 2: Core Types and Concepts</t>
+  </si>
+  <si>
+    <t>Function Return Types and Void</t>
+  </si>
+  <si>
+    <t>Functions as Types</t>
+  </si>
+  <si>
+    <t>Function Types and Callback</t>
+  </si>
+  <si>
+    <t>Quiz 3: Functions &amp; types</t>
+  </si>
+  <si>
+    <t>The 'unknown' type</t>
+  </si>
+  <si>
+    <t>the 'never' type</t>
+  </si>
+  <si>
+    <t>Wrap Up</t>
+  </si>
+  <si>
+    <t>Usefull Resources and links</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,8 +483,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,8 +511,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -449,12 +541,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -463,13 +592,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -754,165 +892,317 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="39.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="10" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="10" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="B12" s="9" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="13" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A12:A37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" location="overview" xr:uid="{A7EFE1D9-B2C6-43E7-B7A5-60F6B186FD75}"/>

</xml_diff>

<commit_message>
Node + Express + Typescript
</commit_message>
<xml_diff>
--- a/Typescript.xlsx
+++ b/Typescript.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="269">
   <si>
     <t>Typescript</t>
   </si>
@@ -809,6 +809,24 @@
   </si>
   <si>
     <t>Working with pops and types of props</t>
+  </si>
+  <si>
+    <t>Executing Typescript Code with Node.JS</t>
+  </si>
+  <si>
+    <t>Setting Up a Project</t>
+  </si>
+  <si>
+    <t>Finished Setup &amp; Working with Types (In NodeJS + Express)</t>
+  </si>
+  <si>
+    <t>Adding Middleware and Types</t>
+  </si>
+  <si>
+    <t>Working with Controllers and Parsing with Request Bodies</t>
+  </si>
+  <si>
+    <t>More CRUD Operations</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1310,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,11 +1321,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B211"/>
+  <dimension ref="A1:B220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A196" sqref="A196:B208"/>
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A210" sqref="A210:B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2518,18 +2536,70 @@
         <v>186</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
-      <c r="A210" s="6" t="s">
+    <row r="210" spans="1:2">
+      <c r="A210" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="6" t="s">
+      <c r="B210" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="14"/>
+      <c r="B211" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="14"/>
+      <c r="B212" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="14"/>
+      <c r="B213" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="14"/>
+      <c r="B214" s="12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="14"/>
+      <c r="B215" s="12" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="14"/>
+      <c r="B216" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" s="14"/>
+      <c r="B217" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" s="15"/>
+      <c r="B218" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="6" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="A210:A218"/>
     <mergeCell ref="A196:A208"/>
     <mergeCell ref="A187:A194"/>
     <mergeCell ref="A179:A185"/>

</xml_diff>